<commit_message>
Added total velocity to the local position and local position setpoint fields.  Added setpoints of the speed and altitude to the automatic plot functions
</commit_message>
<xml_diff>
--- a/CustomPlots/power_and_altitude.xlsx
+++ b/CustomPlots/power_and_altitude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS3_bsp_px4\CustomPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918057E5-C206-4897-AD18-83BA2F26F3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11912B9D-203E-44F9-8E53-1B2976C9C669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>KSID Custom Plot Definition</t>
   </si>
@@ -141,9 +141,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>vehicle_gps_position_0/vel_m_s</t>
-  </si>
-  <si>
     <t>Altitude~[~m~]</t>
   </si>
   <si>
@@ -175,6 +172,21 @@
   </si>
   <si>
     <t>Ground~Speed</t>
+  </si>
+  <si>
+    <t>vehicle_local_position_setpoint_0/v</t>
+  </si>
+  <si>
+    <t>vehicle_local_position_0/v</t>
+  </si>
+  <si>
+    <t>Target~Speed</t>
+  </si>
+  <si>
+    <t>vehicle_local_position_setpoint_0/z</t>
+  </si>
+  <si>
+    <t>Target~Altitude</t>
   </si>
 </sst>
 </file>
@@ -538,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7D595D-48C5-5044-8E94-F6ADF0970571}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -576,7 +588,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3">
         <f>1920-200</f>
@@ -660,19 +672,19 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="O6">
         <v>-1</v>
       </c>
       <c r="R6" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="S6" t="s">
         <v>33</v>
@@ -680,13 +692,13 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
@@ -695,27 +707,27 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
       </c>
       <c r="K7" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="R7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="S7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -730,33 +742,33 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O8">
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
@@ -771,16 +783,16 @@
         <v>24</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -800,19 +812,19 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="S10" t="s">
         <v>34</v>
@@ -820,13 +832,13 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
@@ -835,29 +847,93 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
       </c>
       <c r="K11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>26</v>
+      </c>
+      <c r="S12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
         <v>42</v>
       </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="S13" t="s">
         <v>43</v>
       </c>
-      <c r="S11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
@@ -870,6 +946,12 @@
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>